<commit_message>
added paged numbers to pinyin
</commit_message>
<xml_diff>
--- a/ceremonies/參（辭）駕禮.xlsx
+++ b/ceremonies/參（辭）駕禮.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Xepht\Documents\Xepht\Scripts\Temple\phonetic guide\ceremonies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A0166D-8D14-4E86-8544-5F56C369A75A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E390F2F1-FEDF-4FFB-AD4E-9A1C55F976A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{DF0FECF8-C99E-4A21-9030-3C0ACF01A9BD}"/>
   </bookViews>
@@ -159,24 +159,6 @@
     <t>center</t>
   </si>
   <si>
-    <t>向點傳師參（辭）駕</t>
-  </si>
-  <si>
-    <t>xiàng diǎn chuán shī cān  cí  jià</t>
-  </si>
-  <si>
-    <t>向諸位點傳師接（送）駕</t>
-  </si>
-  <si>
-    <t>xiàng zhū wèi diǎn chuán shī jiē  sòng  jià</t>
-  </si>
-  <si>
-    <t>向點傳師接（送）駕</t>
-  </si>
-  <si>
-    <t>xiàng diǎn chuán shī jiē  sòng  jià</t>
-  </si>
-  <si>
     <t>起作揖</t>
   </si>
   <si>
@@ -189,18 +171,6 @@
     <t>cān  cí  jià lǐ bì chuí shǒu jū gōng</t>
   </si>
   <si>
-    <t>向諸位點傳師參接（辭送）駕</t>
-  </si>
-  <si>
-    <t>xiàng zhū wèi diǎn chuán shī cān jiē  cí sòng  jià</t>
-  </si>
-  <si>
-    <t>向諸位點傳師參（辭）駕</t>
-  </si>
-  <si>
-    <t>xiàng zhū wèi diǎn chuán shī cān  cí  jià</t>
-  </si>
-  <si>
     <t>zhuyin</t>
   </si>
   <si>
@@ -258,22 +228,52 @@
     <t>ㄘㄢ  ㄘˊ  ㄐㄧㄚ` ㄌㄧˇ</t>
   </si>
   <si>
-    <t>ㄒㄧㄤ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄘㄢ  ㄘˊ  ㄐㄧㄚ`</t>
-  </si>
-  <si>
-    <t>ㄒㄧㄤ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄐㄧㄝ  ㄙㄨㄥ`  ㄐㄧㄚ`</t>
-  </si>
-  <si>
-    <t>ㄒㄧㄤ` ㄓㄨ ㄨㄟ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄘㄢ  ㄘˊ  ㄐㄧㄚ`</t>
-  </si>
-  <si>
-    <t>ㄒㄧㄤ` ㄓㄨ ㄨㄟ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄐㄧㄝ  ㄙㄨㄥ`  ㄐㄧㄚ`</t>
-  </si>
-  <si>
-    <t>ㄒㄧㄤ` ㄓㄨ ㄨㄟ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄘㄢ ㄐㄧㄝ  ㄘˊ ㄙㄨㄥ`  ㄐㄧㄚ`</t>
-  </si>
-  <si>
     <t>ㄘㄢ  ㄘˊ  ㄐㄧㄚ` ㄌㄧˇ ㄅㄧ` ㄔㄨㄟˊ ㄕㄡˇ ㄐㄩ ㄍㄨㄥ</t>
+  </si>
+  <si>
+    <t>　向點傳師參（辭）駕</t>
+  </si>
+  <si>
+    <t>　向點傳師接（送）駕</t>
+  </si>
+  <si>
+    <t>　向諸位點傳師參（辭）駕</t>
+  </si>
+  <si>
+    <t>　向諸位點傳師接（送）駕</t>
+  </si>
+  <si>
+    <t>　向諸位點傳師參接（辭送）駕</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xiàng diǎn chuán shī cān  cí  jià</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xiàng diǎn chuán shī jiē  sòng  jià</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xiàng zhū wèi diǎn chuán shī cān  cí  jià</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xiàng zhū wèi diǎn chuán shī jiē  sòng  jià</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xiàng zhū wèi diǎn chuán shī cān jiē  cí sòng  jià</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ㄒㄧㄤ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄘㄢ  ㄘˊ  ㄐㄧㄚ`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ㄒㄧㄤ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄐㄧㄝ  ㄙㄨㄥ`  ㄐㄧㄚ`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ㄒㄧㄤ` ㄓㄨ ㄨㄟ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄘㄢ  ㄘˊ  ㄐㄧㄚ`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ㄒㄧㄤ` ㄓㄨ ㄨㄟ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄐㄧㄝ  ㄙㄨㄥ`  ㄐㄧㄚ`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ㄒㄧㄤ` ㄓㄨ ㄨㄟ` ㄉㄧㄢˇ ㄔㄨㄢˊ ㄕ ㄘㄢ ㄐㄧㄝ  ㄘˊ ㄙㄨㄥ`  ㄐㄧㄚ`</t>
   </si>
 </sst>
 </file>
@@ -629,7 +629,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -757,7 +757,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -825,7 +825,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -876,7 +876,7 @@
         <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +893,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
         <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
         <v>33</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>27</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
         <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
         <v>29</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>33</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>31</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
         <v>33</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1091,13 +1091,13 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
         <v>33</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1125,13 +1125,13 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
         <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1159,13 +1159,13 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>33</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1193,13 +1193,13 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
         <v>33</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1227,13 +1227,13 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>33</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1261,13 +1261,13 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,13 +1278,13 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>